<commit_message>
v0.1 PCB HW work-around
</commit_message>
<xml_diff>
--- a/PCB/BOM.xlsx
+++ b/PCB/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyData\Geek Stuff\Projects\Commodore 64\Hardware\Expansion Port\TeensyROM\TeensyROM\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1BEB401-76F2-4B03-B152-1F0634120BB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1A05610-A37F-4D78-9C51-B28D9B521D9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{5596D14A-B5AE-4503-9066-038068479CCD}"/>
+    <workbookView xWindow="600" yWindow="-14370" windowWidth="19740" windowHeight="11670" activeTab="1" xr2:uid="{5596D14A-B5AE-4503-9066-038068479CCD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="80">
   <si>
     <t>Part</t>
   </si>
@@ -274,6 +274,9 @@
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>Used 22uF</t>
   </si>
 </sst>
 </file>
@@ -1047,10 +1050,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF206551-7640-46D5-B880-F3B0BFEA8EA5}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1084,100 +1087,106 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>75</v>
       </c>
       <c r="D2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="C3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D3" t="s">
-        <v>44</v>
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
+        <v>16</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
+      </c>
+      <c r="D5" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="1">
-        <v>2</v>
+      <c r="A6" s="2">
+        <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="C6" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="D6" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="2">
-        <v>1</v>
+      <c r="A7" s="1">
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="C7" t="s">
-        <v>53</v>
+        <v>71</v>
       </c>
       <c r="D7" t="s">
-        <v>53</v>
+        <v>29</v>
+      </c>
+      <c r="E7" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C8" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="E8" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1185,16 +1194,16 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C9" t="s">
-        <v>73</v>
+        <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="E9" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1202,29 +1211,12 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="1">
-        <v>1</v>
-      </c>
-      <c r="B11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>